<commit_message>
Added some more, bringing the total count to 90
</commit_message>
<xml_diff>
--- a/Batals.xlsx
+++ b/Batals.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{35360BEA-363C-1541-82CC-7BAB1313435A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{766E6B3B-B92D-5840-A5BA-1BC44650C675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="184">
   <si>
     <t>batal</t>
   </si>
@@ -460,6 +460,126 @@
   </si>
   <si>
     <t>بے کار ءُ ناشریں مردم ءَ راکس دوست نہ داریت</t>
+  </si>
+  <si>
+    <t>مرد پہ کار ءُ جہد، نیکہ دستاں بہ بند بہ بوزان پہ زان</t>
+  </si>
+  <si>
+    <t>بیگار مہ بو، بیکار مہ بو۔</t>
+  </si>
+  <si>
+    <t>بیمار ءِ حال پُرسی خداءِ حال پُرسی اِنت، سواب اِنت، بیمار ءِ کرّا بیمار ءَ دلبڈی دیاں، آئی دل ءَ کمزور نہ کن انت</t>
+  </si>
+  <si>
+    <t>بیمار ءِ دل ءَ دور مہ دئے۔</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کس نہ زانت کہ کجام وہد ءَ بیماری کاینت، آ چہ اللہ ءِ نیمگ ءَ </t>
+  </si>
+  <si>
+    <t>بیماری کسی انتظار ءَ نہ کنت۔</t>
+  </si>
+  <si>
+    <t>آ چیز کہ کسان اِنت چہ کسانی ءَ آئی سرا بِہ گر، بیماری بیت یا کہ زہگے بیت، دست ءَ کہ روت گڑا پشومانی کار نہ دنت</t>
+  </si>
+  <si>
+    <t>بیماری ءُ غم ءَ دیر مہ دار۔</t>
+  </si>
+  <si>
+    <t>بیماری ءُ کار کسی لحاظ ءَ نہ کنت۔</t>
+  </si>
+  <si>
+    <t>بیماری چہ خدائی نیمگ ءَ کاینت، کار چہ خدا بنت، اے کسی لحاظ ءَ نہ کن انت۔</t>
+  </si>
+  <si>
+    <t>ہمک کار ءِ سرا ہما وہد امءَ بہ گر</t>
+  </si>
+  <si>
+    <t>بیماری ءَ بے درمان مہ کن۔</t>
+  </si>
+  <si>
+    <t>کسے ءَ را کہ براس نیست بے وس، بے کس نا وس بیت، چنکس کہ مالدار بہ بئے، بلے بے براسی‌گران اِنت</t>
+  </si>
+  <si>
+    <t>بے براسی نا وسی، بے کسی، بے وسی۔</t>
+  </si>
+  <si>
+    <t>زہر ءُ ترندیں گپ دیوان ءَ حراب‌کنت</t>
+  </si>
+  <si>
+    <t>بےبراہ ایں گپ مجلس ءَ مرداکنت۔</t>
+  </si>
+  <si>
+    <t>بے ننگیں مردم ءَ راکسی غیرت نہ گیپت</t>
+  </si>
+  <si>
+    <t>بےپِس ءَ نہ پیرک داریت نہ پِس۔</t>
+  </si>
+  <si>
+    <t>ناتپاکی وت بربادی ے، کسے کہ  ناتپاک بوت گڑا آباد نہ بیت</t>
+  </si>
+  <si>
+    <t>بے تپاکی ہلاکی۔</t>
+  </si>
+  <si>
+    <t>جان دزّ ءُ جان بڈّ لنگڑ بیت</t>
+  </si>
+  <si>
+    <t>بے جان بے نان بیت۔</t>
+  </si>
+  <si>
+    <t>آکہ بے دین اِنت آئی رزق ءِ تہابرکت مان نہ بیت</t>
+  </si>
+  <si>
+    <t>بے دین ءِ رزق برکت نہ کنت۔</t>
+  </si>
+  <si>
+    <t>بے زرّ ءَ راگرّ اِنت ، کسّے وتی نہ کنت</t>
+  </si>
+  <si>
+    <t>بے زَرّی گَرّے۔</t>
+  </si>
+  <si>
+    <t>آ کہ بے سما اِنت، آئی ءَ را پہ گُشگ ءَ ہچ نہ بیت</t>
+  </si>
+  <si>
+    <t>بے سُد پہ پنت ءُ نصحیت ءَ سُد نہ کنت۔</t>
+  </si>
+  <si>
+    <t>آ شہر کہ گوں تئی تالہ ءَ نہ ٹئیت گڑا لَڈّ ءُ بار بہ کن</t>
+  </si>
+  <si>
+    <t>بے سریں شہر ءَ مہ نند۔</t>
+  </si>
+  <si>
+    <t>آ کار ءُ چیز کہ تاوان دینت آ یانی سر امہلہ بہ گر کہ تاوان دنت، آزہگے بہ بیت یا کہ نادراہی ے</t>
+  </si>
+  <si>
+    <t>بے سریں کار ءِ سر ءَ بہ گر۔</t>
+  </si>
+  <si>
+    <t>بے ننگ ءُ بے ضمیریں مردم ءَ نوکر مہ کن</t>
+  </si>
+  <si>
+    <t>بے سریں مرد ءَ نوکر مہ کن۔</t>
+  </si>
+  <si>
+    <t>جاہ ئے کہ روئے توشگ بہ زور، بے سلاح ءُ شور ءَ، بے سرپدی ءُ زانتکاری ءَ حبر مہ کن</t>
+  </si>
+  <si>
+    <t>بے سِلاح ءَ سپر مہ کن، بے صلاح ءَ حبر مہ کن۔</t>
+  </si>
+  <si>
+    <t>ہر چیز ءِ تہا انصاپ بہ بیت، بے تور ءَ تور مہ کن وتی قیامت ءَ کوار مہ کن</t>
+  </si>
+  <si>
+    <t>بے شاہیم ءَ تول نہ بیت۔</t>
+  </si>
+  <si>
+    <t>کول ءُ کرار گوں شوق ءَ بیت، گوں پہکیں مہر ءَ بیت</t>
+  </si>
+  <si>
+    <t>بے شوق ءَ کول نہ بیت۔</t>
   </si>
 </sst>
 </file>
@@ -827,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C74"/>
+  <dimension ref="A1:C95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1617,19 +1737,244 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="2"/>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
+      <c r="A72" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="2"/>
-      <c r="B73" s="2"/>
-      <c r="C73" s="2"/>
+      <c r="A73" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="2"/>
-      <c r="B74" s="2"/>
-      <c r="C74" s="2"/>
+      <c r="A74" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="B76" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C76" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C91" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2"/>
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="2"/>
+      <c r="B94" s="2"/>
+      <c r="C94" s="2"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="2"/>
+      <c r="B95" s="2"/>
+      <c r="C95" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added some more, bringing the total count to 108
</commit_message>
<xml_diff>
--- a/Batals.xlsx
+++ b/Batals.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{766E6B3B-B92D-5840-A5BA-1BC44650C675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1000001_{7F046566-CEF9-894C-809A-5E16A436475A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="220">
   <si>
     <t>batal</t>
   </si>
@@ -580,6 +580,111 @@
   </si>
   <si>
     <t>بے شوق ءَ کول نہ بیت۔</t>
+  </si>
+  <si>
+    <t>بےعزّت ہر جاہ بے عزّت اِنت آنہ وتی عزّت ءَ زانت نیکہ دگرءِ</t>
+  </si>
+  <si>
+    <t>بے عزّت دگر ءَ بے عزّت کنت۔</t>
+  </si>
+  <si>
+    <t>کسے کہ کار نہ کنت، جہد نہ کنت بے بہر اِنت، پَشت کپیت</t>
+  </si>
+  <si>
+    <t>بےکاری، بے بہری۔</t>
+  </si>
+  <si>
+    <t>بےکاریں مردم ہچیز ءِتہانپ نہ گندیت</t>
+  </si>
+  <si>
+    <t>بےکاری، نَپَ نہ داری۔</t>
+  </si>
+  <si>
+    <t>بےکمال ءَ را ہچیز ءِ پرواہ نہ بیت</t>
+  </si>
+  <si>
+    <t>بےکمال نہ سیال گندیت نہ مال۔</t>
+  </si>
+  <si>
+    <t>اگاں کسے ترا لوٹیت دعوت کنت گڑا برو، بے لوٹگ ءَ وتارابے شرپ مہ کن</t>
+  </si>
+  <si>
+    <t>بےلوٹگ ءَ کسی نان ءَ مرو۔</t>
+  </si>
+  <si>
+    <t>بےمال مال نہ کٹیت۔</t>
+  </si>
+  <si>
+    <t>بے جوہر ءُ تاوان ہچ کرت نہ کنت گڑا مال ءَ کجا چہ کٹیت</t>
+  </si>
+  <si>
+    <t>بے مال ءَ را سیال نہ بیت۔</t>
+  </si>
+  <si>
+    <t>بے مال ءُ گریب ءَ کس وتی سیال نہ کنت، دنیا لالچی اِنت</t>
+  </si>
+  <si>
+    <t>بے مالی بدحالی۔</t>
+  </si>
+  <si>
+    <t>آئی ءَ کہ مال نہ بوت بزاں ہچ نہ بوت، بدحالی اِنت</t>
+  </si>
+  <si>
+    <t>مال کہ نہ بوت بدحال بئے</t>
+  </si>
+  <si>
+    <t>بے میاری پہ بلوچ ءَ نبرازی۔</t>
+  </si>
+  <si>
+    <t>بلوچ میار جلیں ننگ داریں راجے آئی واستہ بے میاری عیب اِنت</t>
+  </si>
+  <si>
+    <t>بے میار ءَ راپَیزنبی۔</t>
+  </si>
+  <si>
+    <t>بے لج ءُ ننگ ءِ درور آپ ءِ لکیر کشگ</t>
+  </si>
+  <si>
+    <t>بے ایمان بے نان بیت</t>
+  </si>
+  <si>
+    <t>بےنان بےایمان بیت۔</t>
+  </si>
+  <si>
+    <t>بے نمازی بے روزی، تنگ نمازی تنگ روزی۔</t>
+  </si>
+  <si>
+    <t>کسے ءِ تہا کہ دین نہ بیت، نماز نہ کنت گڑا آئی کِرّا‌ روزی نئیت تنگ بیت</t>
+  </si>
+  <si>
+    <t>بے واہگ ءِ ہمسائگ مہ بو۔</t>
+  </si>
+  <si>
+    <t>اَچ کسے ءَ چہ تماہ نہ گند ئے، واہشت نہ گند ئے وتارا بے شرف مہ کن پہ آئی مرہ، بے واہگیں مردم ءِ همسایگی اوں وش نہ اِنت</t>
+  </si>
+  <si>
+    <t>بے واہگ پہ گلِگ ءَ جوان نہ بیت۔</t>
+  </si>
+  <si>
+    <t>آکہ بے واہگ ءُ ناامیت اِنت آچ آئی ءَ گلِگ کنگ بے نپ اِنت</t>
+  </si>
+  <si>
+    <t>بے وفا نبی سپا۔</t>
+  </si>
+  <si>
+    <t>غدار ءُ دھوکہ باز، ہچبر نہ بنت پارسا</t>
+  </si>
+  <si>
+    <t>بے وفا نگندی نپ ءَ۔</t>
+  </si>
+  <si>
+    <t>آمردم کہ دغاباز اِنت بے وفا اِنت آ ہچبر سیت ءُ نپ نہ گندیت</t>
+  </si>
+  <si>
+    <t>بے ہمتی، بد قسمتی۔</t>
+  </si>
+  <si>
+    <t>کسے کہ جہد نہ کنت، ہمت نہ کنت گڑا شومی کجام بہ بیت</t>
   </si>
 </sst>
 </file>
@@ -947,10 +1052,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C95"/>
+  <dimension ref="A1:C113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A91" sqref="A91"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1957,24 +2062,222 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="2"/>
-      <c r="B92" s="2"/>
-      <c r="C92" s="2"/>
+      <c r="A92" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
+      <c r="A93" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="2"/>
-      <c r="B94" s="2"/>
-      <c r="C94" s="2"/>
+      <c r="A94" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C94" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="2"/>
-      <c r="B95" s="2"/>
-      <c r="C95" s="2"/>
+      <c r="A95" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C95" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="B97" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="B98" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C99" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B102" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C102" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B103" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C103" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C104" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C105" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="B107" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C107" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B108" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C108" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="B109" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C109" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="2"/>
+      <c r="B110" s="2"/>
+      <c r="C110" s="2"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="2"/>
+      <c r="B111" s="2"/>
+      <c r="C111" s="2"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="2"/>
+      <c r="B112" s="2"/>
+      <c r="C112" s="2"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="2"/>
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>